<commit_message>
Actualización última compra en mactrónica
</commit_message>
<xml_diff>
--- a/Lista_componentes.xlsx
+++ b/Lista_componentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegofigueroa/Documents/GitHub/RemoteTempMonitor/PCB_Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Documents\GitHub\RemoteTempMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB75F5C-32E4-3543-980B-771A5DCDE261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4EA7F9-7F39-431B-AFAC-C1E5830EE391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{06313240-559F-D04A-8DD7-FFF8CB69C591}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{06313240-559F-D04A-8DD7-FFF8CB69C591}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
   <si>
     <t>Item</t>
   </si>
@@ -310,18 +310,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -332,12 +326,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,17 +389,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -421,6 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +430,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -741,27 +728,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A532B50-098F-2142-9F42-C1BD222C66BC}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.375" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="3" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" customWidth="1"/>
-    <col min="13" max="13" width="25.1640625" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.125" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="15.875" customWidth="1"/>
+    <col min="9" max="9" width="12.625" customWidth="1"/>
+    <col min="12" max="12" width="16.375" customWidth="1"/>
+    <col min="13" max="13" width="25.125" customWidth="1"/>
+    <col min="14" max="14" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +786,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -838,7 +825,7 @@
         <v>380.8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -877,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -893,7 +880,7 @@
       <c r="E4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -910,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -923,27 +910,33 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="E5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1">
+        <v>1500</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="J5" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>-4500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -956,27 +949,33 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="J6" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1016,7 +1015,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1026,7 +1025,7 @@
       <c r="C8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1056,7 +1055,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1069,10 +1068,10 @@
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="1">
         <v>0</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1108,27 +1107,33 @@
       <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1">
+        <v>25000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="J10" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1141,7 +1146,7 @@
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="2"/>
@@ -1167,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1180,7 +1185,7 @@
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F12" s="2"/>
@@ -1206,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1245,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1285,7 +1290,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1324,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1363,7 +1368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1402,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1442,7 +1447,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1452,7 +1457,7 @@
       <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1481,7 +1486,7 @@
         <v>535.5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1491,7 +1496,7 @@
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>70</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1520,7 +1525,7 @@
         <v>535.5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1559,7 +1564,7 @@
         <v>190.4</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1598,7 +1603,7 @@
         <v>380.8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1637,7 +1642,7 @@
         <v>333.2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1676,7 +1681,7 @@
         <v>428.40000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1715,7 +1720,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1755,7 +1760,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1794,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1833,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1873,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1886,27 +1891,33 @@
       <c r="D30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="E30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="1">
+        <v>1500</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="J30" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M30" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1945,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1983,27 +1994,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
       <c r="J33" s="1">
         <f>SUM(J2:J32)</f>
-        <v>73364</v>
+        <v>103364</v>
       </c>
       <c r="M33" s="1">
         <f>SUM(M2:M32)</f>
-        <v>5283.6</v>
-      </c>
-    </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D37" s="10" t="s">
+        <v>783.60000000000025</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D37" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="11"/>
-      <c r="G37" s="12" t="s">
+      <c r="E37" s="9"/>
+      <c r="G37" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="H37" s="12"/>
-    </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D38" s="1" t="s">
         <v>61</v>
       </c>
@@ -2019,7 +2030,7 @@
         <v>42364</v>
       </c>
     </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D39" s="1" t="s">
         <v>62</v>
       </c>
@@ -2032,16 +2043,16 @@
       </c>
       <c r="H39" s="1">
         <f>SUMIF(E2:E31,"Mactrónica",J2:J31)</f>
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.2">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D40" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E40" s="1">
         <f>SUMIF(I2:I32,"Danny",J2:J32)</f>
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>50</v>
@@ -2051,10 +2062,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E41" s="1">
         <f>SUM(E38:E40)</f>
-        <v>73364</v>
+        <v>103364</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>66</v>
@@ -2064,10 +2075,10 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H42" s="1">
         <f>SUM(H38:H41)</f>
-        <v>73364</v>
+        <v>103364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización con precios de las baterías
</commit_message>
<xml_diff>
--- a/Lista_componentes.xlsx
+++ b/Lista_componentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Documents\GitHub\RemoteTempMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4EA7F9-7F39-431B-AFAC-C1E5830EE391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025941F7-B8D9-4A46-9AEC-91252ED9DC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{06313240-559F-D04A-8DD7-FFF8CB69C591}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
   <si>
     <t>Item</t>
   </si>
@@ -310,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,12 +320,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,15 +383,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -407,7 +401,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A532B50-098F-2142-9F42-C1BD222C66BC}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -880,21 +873,27 @@
       <c r="E4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4">
+      <c r="F4" s="5"/>
+      <c r="G4" s="6">
+        <v>35800</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="6">
         <f t="shared" ref="J4:J32" si="2">G4*H4</f>
-        <v>0</v>
+        <v>35800</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-35800</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -910,7 +909,7 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F5" s="2"/>
@@ -949,7 +948,7 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="7" t="s">
         <v>48</v>
       </c>
       <c r="F6" s="2"/>
@@ -959,7 +958,7 @@
       <c r="H6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J6" s="1">
@@ -1025,7 +1024,7 @@
       <c r="C8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1068,10 +1067,10 @@
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="1">
         <v>0</v>
       </c>
@@ -1107,7 +1106,7 @@
       <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="7" t="s">
         <v>48</v>
       </c>
       <c r="F10" s="2"/>
@@ -1146,7 +1145,7 @@
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="2"/>
@@ -1185,7 +1184,7 @@
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F12" s="2"/>
@@ -1457,7 +1456,7 @@
       <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>69</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1496,7 +1495,7 @@
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>70</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1891,7 +1890,7 @@
       <c r="D30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F30" s="2"/>
@@ -1997,11 +1996,11 @@
     <row r="33" spans="4:13" x14ac:dyDescent="0.25">
       <c r="J33" s="1">
         <f>SUM(J2:J32)</f>
-        <v>103364</v>
+        <v>139164</v>
       </c>
       <c r="M33" s="1">
         <f>SUM(M2:M32)</f>
-        <v>783.60000000000025</v>
+        <v>-35016.399999999994</v>
       </c>
     </row>
     <row r="37" spans="4:13" x14ac:dyDescent="0.25">
@@ -2036,7 +2035,7 @@
       </c>
       <c r="E39" s="1">
         <f>SUMIF(I2:I32,"Omar",J2:J32)</f>
-        <v>1000</v>
+        <v>36800</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>48</v>
@@ -2059,13 +2058,13 @@
       </c>
       <c r="H40" s="1">
         <f>SUMIF(E2:E32,"Mercado Libre",J2:J32)</f>
-        <v>0</v>
+        <v>35800</v>
       </c>
     </row>
     <row r="41" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E41" s="1">
         <f>SUM(E38:E40)</f>
-        <v>103364</v>
+        <v>139164</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>66</v>
@@ -2078,7 +2077,7 @@
     <row r="42" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H42" s="1">
         <f>SUM(H38:H41)</f>
-        <v>103364</v>
+        <v>139164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lista de componentes y precios terminada
</commit_message>
<xml_diff>
--- a/Lista_componentes.xlsx
+++ b/Lista_componentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Documents\GitHub\RemoteTempMonitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegofigueroa/Documents/GitHub/RemoteTempMonitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025941F7-B8D9-4A46-9AEC-91252ED9DC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13382D5-F776-F342-8216-CF73F780CCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{06313240-559F-D04A-8DD7-FFF8CB69C591}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{06313240-559F-D04A-8DD7-FFF8CB69C591}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="80">
   <si>
     <t>Item</t>
   </si>
@@ -250,9 +250,6 @@
     <t>cantidad compra</t>
   </si>
   <si>
-    <t>Centro</t>
-  </si>
-  <si>
     <t>0.1u</t>
   </si>
   <si>
@@ -281,6 +278,18 @@
   </si>
   <si>
     <t>Precio de elementos sobrantes</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Envio mercado libre</t>
+  </si>
+  <si>
+    <t>Contacto PCB</t>
+  </si>
+  <si>
+    <t>Saldo</t>
   </si>
 </sst>
 </file>
@@ -330,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -379,11 +388,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -401,12 +423,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7D90"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -423,7 +480,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -719,29 +776,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A532B50-098F-2142-9F42-C1BD222C66BC}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.375" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="3" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.125" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="15.875" customWidth="1"/>
-    <col min="9" max="9" width="12.625" customWidth="1"/>
-    <col min="12" max="12" width="16.375" customWidth="1"/>
-    <col min="13" max="13" width="25.125" customWidth="1"/>
-    <col min="14" max="14" width="13.125" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="27" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,13 +830,13 @@
         <v>59</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -787,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -818,7 +875,7 @@
         <v>380.8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -849,15 +906,15 @@
         <v>10000</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L32" si="0">H3-B3</f>
+        <f t="shared" ref="L3:L34" si="0">H3-B3</f>
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M32" si="1">L3*G3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M3:M34" si="1">L3*G3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -875,28 +932,28 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="6">
-        <v>35800</v>
+        <v>10400</v>
       </c>
       <c r="H4" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>62</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" ref="J4:J32" si="2">G4*H4</f>
-        <v>35800</v>
+        <f t="shared" ref="J4:J34" si="2">G4*H4</f>
+        <v>20800</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" si="1"/>
-        <v>-35800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -914,10 +971,11 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1">
-        <v>1500</v>
+        <f>1500/4</f>
+        <v>375</v>
       </c>
       <c r="H5" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>63</v>
@@ -928,14 +986,14 @@
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="1"/>
-        <v>-4500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -974,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1014,7 +1072,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1025,7 +1083,7 @@
         <v>38</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>47</v>
@@ -1054,7 +1112,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1093,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1132,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1171,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1210,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1249,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1289,7 +1347,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1328,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1367,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1381,7 +1439,7 @@
         <v>64</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="1">
@@ -1406,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1446,7 +1504,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1457,7 +1515,7 @@
         <v>24</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>47</v>
@@ -1485,7 +1543,7 @@
         <v>535.5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1496,7 +1554,7 @@
         <v>25</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>47</v>
@@ -1524,7 +1582,7 @@
         <v>535.5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1563,7 +1621,7 @@
         <v>190.4</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1602,7 +1660,7 @@
         <v>380.8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1641,7 +1699,7 @@
         <v>333.2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1680,7 +1738,7 @@
         <v>428.40000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1719,7 +1777,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1759,7 +1817,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1773,7 +1831,7 @@
         <v>58</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="1">
@@ -1798,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1837,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1877,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1916,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1955,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1963,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="3" t="s">
@@ -1993,98 +2051,208 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12">
+        <v>1</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="12">
+        <v>45000</v>
+      </c>
+      <c r="H33" s="12">
+        <v>1</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="J33" s="1">
-        <f>SUM(J2:J32)</f>
-        <v>139164</v>
+        <f t="shared" si="2"/>
+        <v>45000</v>
+      </c>
+      <c r="L33" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="M33" s="1">
-        <f>SUM(M2:M32)</f>
-        <v>-35016.399999999994</v>
-      </c>
-    </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D37" s="8" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="12">
+        <v>1</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="12">
+        <v>15000</v>
+      </c>
+      <c r="H34" s="12">
+        <v>1</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="2"/>
+        <v>15000</v>
+      </c>
+      <c r="L34" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J35" s="11">
+        <f>SUM(J2:J34)</f>
+        <v>184164</v>
+      </c>
+      <c r="M35" s="1">
+        <f>SUM(M2:M34)</f>
+        <v>5283.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D39" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="9"/>
-      <c r="G37" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H37" s="10"/>
-    </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" s="1">
-        <f>SUMIF(I2:I32,"Diego",J2:J32)</f>
-        <v>72364</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="I39" s="10"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="1">
+        <f>SUMIF(I2:I34,"Diego",J2:J34)</f>
+        <v>117364</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40-$E$43/3</f>
+        <v>55976</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H38" s="1">
-        <f>SUMIF(E2:E32,"Sigma",J2:J32)</f>
+      <c r="I40" s="1">
+        <f>SUMIF(E2:E34,"Sigma",J2:J34)</f>
         <v>42364</v>
       </c>
     </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D39" s="1" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="1">
-        <f>SUMIF(I2:I32,"Omar",J2:J32)</f>
+      <c r="E41" s="1">
+        <f>SUMIF(I2:I34,"Omar",J2:J34)</f>
         <v>36800</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="F41" s="1">
+        <f t="shared" ref="F41:F42" si="3">E41-$E$43/3</f>
+        <v>-24588</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H39" s="1">
-        <f>SUMIF(E2:E31,"Mactrónica",J2:J31)</f>
+      <c r="I41" s="1">
+        <f>SUMIF(E2:E34,"Mactrónica",J2:J34)</f>
         <v>60000</v>
       </c>
     </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D40" s="1" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="1">
-        <f>SUMIF(I2:I32,"Danny",J2:J32)</f>
+      <c r="E42" s="1">
+        <f>SUMIF(I2:I34,"Danny",J2:J34)</f>
         <v>30000</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>-31388</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H40" s="1">
-        <f>SUMIF(E2:E32,"Mercado Libre",J2:J32)</f>
+      <c r="I42" s="1">
+        <f>SUMIF(E2:E34,"Mercado Libre",J2:J34)</f>
         <v>35800</v>
       </c>
     </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="E41" s="1">
-        <f>SUM(E38:E40)</f>
-        <v>139164</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H41" s="1">
-        <f>SUMIF(E2:E32,"Centro",J2:J32)</f>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E43" s="1">
+        <f>SUM(E40:E42)</f>
+        <v>184164</v>
+      </c>
+      <c r="F43" s="1">
+        <f>SUM(F40:F42)</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I43" s="1">
+        <f>SUMIF(E2:E34,"Contacto PCB",J2:J34)</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I44" s="1">
+        <f>SUMIF(E2:E35,"centro",J2:J35)</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="H42" s="1">
-        <f>SUM(H38:H41)</f>
-        <v>139164</v>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I45" s="1">
+        <f>SUM(I40:I44)</f>
+        <v>184164</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H39:I39"/>
   </mergeCells>
+  <conditionalFormatting sqref="F40:F42">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>